<commit_message>
Disabled sliders if it would cause a mixed constraint; worked around floating point roundoff errors
</commit_message>
<xml_diff>
--- a/doc/Logs.xlsx
+++ b/doc/Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RCalc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{408B9226-0C5F-4B85-82D2-8C4A1349D4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3FF46-A1CC-4FAC-B3B1-772D984AD61A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10590" yWindow="1230" windowWidth="18210" windowHeight="12975" xr2:uid="{CD37A0FF-76A3-46D2-B354-CFC531E43072}"/>
   </bookViews>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827BE93C-4892-405F-B6CC-E8BECAF04B76}">
-  <dimension ref="E5:Q31"/>
+  <dimension ref="E3:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +438,11 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2.8999999999999999E-9</v>
+      </c>
+    </row>
     <row r="5" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
         <v>10</v>
@@ -481,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="str">
-        <f>VLOOKUP(H7,$P$7:$Q$15,2)</f>
+        <f t="shared" ref="J7:J31" si="0">VLOOKUP(H7,$P$7:$Q$15,2)</f>
         <v>pico</v>
       </c>
       <c r="L7">
@@ -493,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="str">
-        <f>VLOOKUP(L7,$P$7:$Q$15,2)</f>
+        <f t="shared" ref="N7:N31" si="1">VLOOKUP(L7,$P$7:$Q$15,2)</f>
         <v>pico</v>
       </c>
       <c r="P7">
@@ -508,35 +513,35 @@
         <v>-11</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F31" si="0">10^E8</f>
+        <f t="shared" ref="F8:F31" si="2">10^E8</f>
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G31" si="1">LOG10(F8)</f>
+        <f t="shared" ref="G8:G31" si="3">LOG10(F8)</f>
         <v>-11</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H31" si="2">_xlfn.FLOOR.MATH($G8/3)</f>
+        <f t="shared" ref="H8:H31" si="4">_xlfn.FLOOR.MATH($G8/3)</f>
         <v>-4</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I31" si="3">$F8/(10^(3*H8))</f>
+        <f t="shared" ref="I8:I31" si="5">$F8/(10^(3*H8))</f>
         <v>10</v>
       </c>
       <c r="J8" t="str">
-        <f>VLOOKUP(H8,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>pico</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L31" si="4">_xlfn.CEILING.MATH($G8/3)</f>
+        <f t="shared" ref="L8:L31" si="6">_xlfn.CEILING.MATH($G8/3)</f>
         <v>-3</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M31" si="5">$F8/(10^(3*L8))</f>
+        <f t="shared" ref="M8:M31" si="7">$F8/(10^(3*L8))</f>
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="N8" t="str">
-        <f>VLOOKUP(L8,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nano</v>
       </c>
       <c r="P8">
@@ -551,35 +556,35 @@
         <v>-10</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1E-10</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J9" t="str">
-        <f>VLOOKUP(H9,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>pico</v>
       </c>
       <c r="L9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="N9" t="str">
-        <f>VLOOKUP(L9,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nano</v>
       </c>
       <c r="P9">
@@ -594,35 +599,35 @@
         <v>-9</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J10" t="str">
-        <f>VLOOKUP(H10,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>nano</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N10" t="str">
-        <f>VLOOKUP(L10,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nano</v>
       </c>
       <c r="P10">
@@ -637,35 +642,35 @@
         <v>-8</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1E-8</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J11" t="str">
-        <f>VLOOKUP(H11,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>nano</v>
       </c>
       <c r="L11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N11" t="str">
-        <f>VLOOKUP(L11,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>micro</v>
       </c>
       <c r="P11">
@@ -680,35 +685,35 @@
         <v>-7</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-7</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.999999999999986</v>
       </c>
       <c r="J12" t="str">
-        <f>VLOOKUP(H12,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>nano</v>
       </c>
       <c r="L12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N12" t="str">
-        <f>VLOOKUP(L12,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>micro</v>
       </c>
       <c r="P12">
@@ -723,35 +728,35 @@
         <v>-6</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J13" t="str">
-        <f>VLOOKUP(H13,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>micro</v>
       </c>
       <c r="L13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N13" t="str">
-        <f>VLOOKUP(L13,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>micro</v>
       </c>
       <c r="P13">
@@ -766,35 +771,35 @@
         <v>-5</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10.000000000000002</v>
       </c>
       <c r="J14" t="str">
-        <f>VLOOKUP(H14,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>micro</v>
       </c>
       <c r="L14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N14" t="str">
-        <f>VLOOKUP(L14,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>milli</v>
       </c>
       <c r="P14">
@@ -809,35 +814,35 @@
         <v>-4</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1E-4</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100.00000000000001</v>
       </c>
       <c r="J15" t="str">
-        <f>VLOOKUP(H15,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>micro</v>
       </c>
       <c r="L15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N15" t="str">
-        <f>VLOOKUP(L15,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>milli</v>
       </c>
       <c r="P15">
@@ -852,35 +857,35 @@
         <v>-3</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="I16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J16" t="str">
-        <f>VLOOKUP(H16,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>milli</v>
       </c>
       <c r="L16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="M16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N16" t="str">
-        <f>VLOOKUP(L16,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>milli</v>
       </c>
     </row>
@@ -889,35 +894,35 @@
         <v>-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J17" t="str">
-        <f>VLOOKUP(H17,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>milli</v>
       </c>
       <c r="L17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N17" t="str">
-        <f>VLOOKUP(L17,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>normal</v>
       </c>
     </row>
@@ -926,35 +931,35 @@
         <v>-1</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J18" t="str">
-        <f>VLOOKUP(H18,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>milli</v>
       </c>
       <c r="L18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N18" t="str">
-        <f>VLOOKUP(L18,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>normal</v>
       </c>
     </row>
@@ -963,35 +968,35 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J19" t="str">
-        <f>VLOOKUP(H19,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>normal</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N19" t="str">
-        <f>VLOOKUP(L19,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>normal</v>
       </c>
     </row>
@@ -1000,35 +1005,35 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J20" t="str">
-        <f>VLOOKUP(H20,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>normal</v>
       </c>
       <c r="L20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N20" t="str">
-        <f>VLOOKUP(L20,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>kilo</v>
       </c>
     </row>
@@ -1037,35 +1042,35 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J21" t="str">
-        <f>VLOOKUP(H21,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>normal</v>
       </c>
       <c r="L21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N21" t="str">
-        <f>VLOOKUP(L21,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>kilo</v>
       </c>
     </row>
@@ -1074,35 +1079,35 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J22" t="str">
-        <f>VLOOKUP(H22,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>kilo</v>
       </c>
       <c r="L22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N22" t="str">
-        <f>VLOOKUP(L22,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>kilo</v>
       </c>
     </row>
@@ -1111,35 +1116,35 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J23" t="str">
-        <f>VLOOKUP(H23,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>kilo</v>
       </c>
       <c r="L23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N23" t="str">
-        <f>VLOOKUP(L23,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>mega</v>
       </c>
     </row>
@@ -1148,35 +1153,35 @@
         <v>5</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100000</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J24" t="str">
-        <f>VLOOKUP(H24,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>kilo</v>
       </c>
       <c r="L24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N24" t="str">
-        <f>VLOOKUP(L24,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>mega</v>
       </c>
     </row>
@@ -1185,35 +1190,35 @@
         <v>6</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J25" t="str">
-        <f>VLOOKUP(H25,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>mega</v>
       </c>
       <c r="L25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N25" t="str">
-        <f>VLOOKUP(L25,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>mega</v>
       </c>
     </row>
@@ -1222,35 +1227,35 @@
         <v>7</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J26" t="str">
-        <f>VLOOKUP(H26,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>mega</v>
       </c>
       <c r="L26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="M26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N26" t="str">
-        <f>VLOOKUP(L26,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>giga</v>
       </c>
     </row>
@@ -1259,35 +1264,35 @@
         <v>8</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100000000</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J27" t="str">
-        <f>VLOOKUP(H27,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>mega</v>
       </c>
       <c r="L27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="M27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N27" t="str">
-        <f>VLOOKUP(L27,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>giga</v>
       </c>
     </row>
@@ -1296,35 +1301,35 @@
         <v>9</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000000000</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J28" t="str">
-        <f>VLOOKUP(H28,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>giga</v>
       </c>
       <c r="L28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="M28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N28" t="str">
-        <f>VLOOKUP(L28,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>giga</v>
       </c>
     </row>
@@ -1333,35 +1338,35 @@
         <v>10</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10000000000</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J29" t="str">
-        <f>VLOOKUP(H29,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>giga</v>
       </c>
       <c r="L29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="M29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="N29" t="str">
-        <f>VLOOKUP(L29,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>tera</v>
       </c>
     </row>
@@ -1370,35 +1375,35 @@
         <v>11</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100000000000</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="J30" t="str">
-        <f>VLOOKUP(H30,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>giga</v>
       </c>
       <c r="L30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="M30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
       <c r="N30" t="str">
-        <f>VLOOKUP(L30,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>tera</v>
       </c>
     </row>
@@ -1407,35 +1412,35 @@
         <v>12</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000000000000</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J31" t="str">
-        <f>VLOOKUP(H31,$P$7:$Q$15,2)</f>
+        <f t="shared" si="0"/>
         <v>tera</v>
       </c>
       <c r="L31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="M31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N31" t="str">
-        <f>VLOOKUP(L31,$P$7:$Q$15,2)</f>
+        <f t="shared" si="1"/>
         <v>tera</v>
       </c>
     </row>

</xml_diff>